<commit_message>
Added support for updating multiple pivot table associations in the ExcelSlicerCache.
</commit_message>
<xml_diff>
--- a/EPPlusTest/Workbooks/SlicerFromExcel.xlsx
+++ b/EPPlusTest/Workbooks/SlicerFromExcel.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\med\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zpf\Documents\DELME\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -22,7 +22,7 @@
   </definedNames>
   <calcPr calcId="162913"/>
   <pivotCaches>
-    <pivotCache cacheId="12" r:id="rId5"/>
+    <pivotCache cacheId="126" r:id="rId5"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{BBE1A952-AA13-448e-AADC-164F8A28A991}">
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1780" uniqueCount="185">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1980" uniqueCount="185">
   <si>
     <t>Hide</t>
   </si>
@@ -646,7 +646,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -656,6 +656,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" indent="2"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -733,13 +739,13 @@
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>647700</xdr:colOff>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
       <xdr:row>15</xdr:row>
       <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:graphicFrame macro="">
           <xdr:nvGraphicFramePr>
             <xdr:cNvPr id="5" name="Description"/>
@@ -756,7 +762,7 @@
           </a:graphic>
         </xdr:graphicFrame>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="0" name=""/>
@@ -896,7 +902,74 @@
       </sharedItems>
     </cacheField>
     <cacheField name="No." numFmtId="49">
-      <sharedItems/>
+      <sharedItems count="66">
+        <s v="70000"/>
+        <s v="70001"/>
+        <s v="70002"/>
+        <s v="70003"/>
+        <s v="70040"/>
+        <s v="70041"/>
+        <s v="70011"/>
+        <s v="70200"/>
+        <s v="70201"/>
+        <s v="1996-S"/>
+        <s v="70103"/>
+        <s v="70100"/>
+        <s v="70010"/>
+        <s v="70102"/>
+        <s v="70101"/>
+        <s v="70104"/>
+        <s v="1920-S"/>
+        <s v="1900-S"/>
+        <s v="1952-W"/>
+        <s v="1928-W"/>
+        <s v="1976-W"/>
+        <s v="1964-W"/>
+        <s v="70060"/>
+        <s v="1896-S"/>
+        <s v="1908-S"/>
+        <s v="1928-S"/>
+        <s v="80001"/>
+        <s v="80010"/>
+        <s v="80201"/>
+        <s v="80021"/>
+        <s v="80101"/>
+        <s v="80206"/>
+        <s v="80211"/>
+        <s v="80002"/>
+        <s v="80011"/>
+        <s v="80202"/>
+        <s v="80023"/>
+        <s v="80102"/>
+        <s v="80208"/>
+        <s v="80209"/>
+        <s v="80003"/>
+        <s v="80013"/>
+        <s v="80024"/>
+        <s v="80103"/>
+        <s v="80212"/>
+        <s v="80004"/>
+        <s v="80014"/>
+        <s v="80203"/>
+        <s v="80026"/>
+        <s v="80204"/>
+        <s v="80105"/>
+        <s v="80207"/>
+        <s v="80210"/>
+        <s v="80213"/>
+        <s v="80214"/>
+        <s v="80027"/>
+        <s v="80205"/>
+        <s v="80006"/>
+        <s v="80007"/>
+        <s v="LSU-15"/>
+        <s v="LSU-8"/>
+        <s v="LSU-4"/>
+        <s v="FF-100"/>
+        <s v="C-100"/>
+        <s v="HS-100"/>
+        <s v="SPK-100"/>
+      </sharedItems>
     </cacheField>
     <cacheField name="Parent Item No." numFmtId="49">
       <sharedItems/>
@@ -907,10 +980,14 @@
       </sharedItems>
     </cacheField>
     <cacheField name="Position 2" numFmtId="49">
-      <sharedItems/>
+      <sharedItems count="1">
+        <s v=""/>
+      </sharedItems>
     </cacheField>
     <cacheField name="Position 3" numFmtId="49">
-      <sharedItems/>
+      <sharedItems count="1">
+        <s v=""/>
+      </sharedItems>
     </cacheField>
     <cacheField name="Quantity per" numFmtId="0">
       <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1" maxValue="12"/>
@@ -955,11 +1032,11 @@
     <x v="0"/>
     <n v="10000"/>
     <x v="0"/>
-    <s v="70000"/>
+    <x v="0"/>
     <s v="1924-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="2"/>
     <x v="0"/>
     <x v="0"/>
@@ -973,11 +1050,11 @@
     <x v="0"/>
     <n v="20000"/>
     <x v="0"/>
-    <s v="70001"/>
+    <x v="1"/>
     <s v="1924-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -991,11 +1068,11 @@
     <x v="0"/>
     <n v="30000"/>
     <x v="0"/>
-    <s v="70002"/>
+    <x v="2"/>
     <s v="1924-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -1009,11 +1086,11 @@
     <x v="0"/>
     <n v="40000"/>
     <x v="0"/>
-    <s v="70003"/>
+    <x v="3"/>
     <s v="1924-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -1027,11 +1104,11 @@
     <x v="0"/>
     <n v="20000"/>
     <x v="0"/>
-    <s v="70000"/>
+    <x v="0"/>
     <s v="1928-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="2"/>
     <x v="0"/>
     <x v="0"/>
@@ -1045,11 +1122,11 @@
     <x v="0"/>
     <n v="30000"/>
     <x v="0"/>
-    <s v="70001"/>
+    <x v="1"/>
     <s v="1928-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -1063,11 +1140,11 @@
     <x v="0"/>
     <n v="40000"/>
     <x v="0"/>
-    <s v="70002"/>
+    <x v="2"/>
     <s v="1928-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -1081,11 +1158,11 @@
     <x v="0"/>
     <n v="50000"/>
     <x v="0"/>
-    <s v="70003"/>
+    <x v="3"/>
     <s v="1928-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -1099,11 +1176,11 @@
     <x v="0"/>
     <n v="60000"/>
     <x v="0"/>
-    <s v="70040"/>
+    <x v="4"/>
     <s v="1928-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="2"/>
     <x v="0"/>
     <x v="0"/>
@@ -1117,11 +1194,11 @@
     <x v="0"/>
     <n v="20000"/>
     <x v="0"/>
-    <s v="70000"/>
+    <x v="0"/>
     <s v="1952-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="2"/>
     <x v="0"/>
     <x v="0"/>
@@ -1135,11 +1212,11 @@
     <x v="0"/>
     <n v="30000"/>
     <x v="0"/>
-    <s v="70001"/>
+    <x v="1"/>
     <s v="1952-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -1153,11 +1230,11 @@
     <x v="0"/>
     <n v="40000"/>
     <x v="0"/>
-    <s v="70002"/>
+    <x v="2"/>
     <s v="1952-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -1171,11 +1248,11 @@
     <x v="0"/>
     <n v="50000"/>
     <x v="0"/>
-    <s v="70003"/>
+    <x v="3"/>
     <s v="1952-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -1189,11 +1266,11 @@
     <x v="0"/>
     <n v="60000"/>
     <x v="0"/>
-    <s v="70041"/>
+    <x v="5"/>
     <s v="1952-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -1207,11 +1284,11 @@
     <x v="0"/>
     <n v="20000"/>
     <x v="0"/>
-    <s v="70000"/>
+    <x v="0"/>
     <s v="1964-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="2"/>
     <x v="0"/>
     <x v="0"/>
@@ -1225,11 +1302,11 @@
     <x v="0"/>
     <n v="30000"/>
     <x v="0"/>
-    <s v="70001"/>
+    <x v="1"/>
     <s v="1964-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -1243,11 +1320,11 @@
     <x v="0"/>
     <n v="40000"/>
     <x v="0"/>
-    <s v="70002"/>
+    <x v="2"/>
     <s v="1964-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -1261,11 +1338,11 @@
     <x v="0"/>
     <n v="50000"/>
     <x v="0"/>
-    <s v="70003"/>
+    <x v="3"/>
     <s v="1964-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -1279,11 +1356,11 @@
     <x v="0"/>
     <n v="60000"/>
     <x v="0"/>
-    <s v="70041"/>
+    <x v="5"/>
     <s v="1964-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -1297,11 +1374,11 @@
     <x v="0"/>
     <n v="70000"/>
     <x v="0"/>
-    <s v="70011"/>
+    <x v="6"/>
     <s v="1964-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="2"/>
     <x v="0"/>
     <x v="0"/>
@@ -1315,11 +1392,11 @@
     <x v="0"/>
     <n v="80000"/>
     <x v="0"/>
-    <s v="70200"/>
+    <x v="7"/>
     <s v="1964-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="4"/>
     <x v="0"/>
     <x v="0"/>
@@ -1333,11 +1410,11 @@
     <x v="0"/>
     <n v="90000"/>
     <x v="0"/>
-    <s v="70201"/>
+    <x v="8"/>
     <s v="1964-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="2"/>
     <x v="0"/>
     <x v="0"/>
@@ -1351,11 +1428,11 @@
     <x v="0"/>
     <n v="20000"/>
     <x v="0"/>
-    <s v="1996-S"/>
+    <x v="9"/>
     <s v="1968-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -1369,11 +1446,11 @@
     <x v="0"/>
     <n v="30000"/>
     <x v="0"/>
-    <s v="70103"/>
+    <x v="10"/>
     <s v="1968-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -1387,11 +1464,11 @@
     <x v="0"/>
     <n v="10000"/>
     <x v="0"/>
-    <s v="1996-S"/>
+    <x v="9"/>
     <s v="1972-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -1405,11 +1482,11 @@
     <x v="0"/>
     <n v="20000"/>
     <x v="0"/>
-    <s v="70100"/>
+    <x v="11"/>
     <s v="1972-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -1423,11 +1500,11 @@
     <x v="0"/>
     <n v="20000"/>
     <x v="0"/>
-    <s v="70000"/>
+    <x v="0"/>
     <s v="1976-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="2"/>
     <x v="0"/>
     <x v="0"/>
@@ -1441,11 +1518,11 @@
     <x v="0"/>
     <n v="30000"/>
     <x v="0"/>
-    <s v="70001"/>
+    <x v="1"/>
     <s v="1976-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -1459,11 +1536,11 @@
     <x v="0"/>
     <n v="40000"/>
     <x v="0"/>
-    <s v="70002"/>
+    <x v="2"/>
     <s v="1976-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -1477,11 +1554,11 @@
     <x v="0"/>
     <n v="50000"/>
     <x v="0"/>
-    <s v="70003"/>
+    <x v="3"/>
     <s v="1976-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -1495,11 +1572,11 @@
     <x v="0"/>
     <n v="60000"/>
     <x v="0"/>
-    <s v="70041"/>
+    <x v="5"/>
     <s v="1976-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -1513,11 +1590,11 @@
     <x v="0"/>
     <n v="70000"/>
     <x v="0"/>
-    <s v="70010"/>
+    <x v="12"/>
     <s v="1976-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="2"/>
     <x v="0"/>
     <x v="0"/>
@@ -1531,11 +1608,11 @@
     <x v="0"/>
     <n v="80000"/>
     <x v="0"/>
-    <s v="70200"/>
+    <x v="7"/>
     <s v="1976-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="4"/>
     <x v="0"/>
     <x v="0"/>
@@ -1549,11 +1626,11 @@
     <x v="0"/>
     <n v="90000"/>
     <x v="0"/>
-    <s v="70201"/>
+    <x v="8"/>
     <s v="1976-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="2"/>
     <x v="0"/>
     <x v="0"/>
@@ -1567,11 +1644,11 @@
     <x v="0"/>
     <n v="20000"/>
     <x v="0"/>
-    <s v="1996-S"/>
+    <x v="9"/>
     <s v="1984-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -1585,11 +1662,11 @@
     <x v="0"/>
     <n v="30000"/>
     <x v="0"/>
-    <s v="70102"/>
+    <x v="13"/>
     <s v="1984-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -1603,11 +1680,11 @@
     <x v="0"/>
     <n v="20000"/>
     <x v="0"/>
-    <s v="1996-S"/>
+    <x v="9"/>
     <s v="1988-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -1621,11 +1698,11 @@
     <x v="0"/>
     <n v="30000"/>
     <x v="0"/>
-    <s v="70101"/>
+    <x v="14"/>
     <s v="1988-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -1639,11 +1716,11 @@
     <x v="0"/>
     <n v="20000"/>
     <x v="0"/>
-    <s v="1996-S"/>
+    <x v="9"/>
     <s v="1992-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -1657,11 +1734,11 @@
     <x v="0"/>
     <n v="30000"/>
     <x v="0"/>
-    <s v="70104"/>
+    <x v="15"/>
     <s v="1992-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -1675,11 +1752,11 @@
     <x v="0"/>
     <n v="10000"/>
     <x v="0"/>
-    <s v="1920-S"/>
+    <x v="16"/>
     <s v="766BC-A"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="5"/>
     <x v="0"/>
     <x v="0"/>
@@ -1693,11 +1770,11 @@
     <x v="0"/>
     <n v="20000"/>
     <x v="0"/>
-    <s v="1900-S"/>
+    <x v="17"/>
     <s v="766BC-A"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="12"/>
     <x v="0"/>
     <x v="0"/>
@@ -1711,11 +1788,11 @@
     <x v="0"/>
     <n v="30000"/>
     <x v="0"/>
-    <s v="1996-S"/>
+    <x v="9"/>
     <s v="766BC-A"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -1729,11 +1806,11 @@
     <x v="0"/>
     <n v="40000"/>
     <x v="0"/>
-    <s v="70102"/>
+    <x v="13"/>
     <s v="766BC-A"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -1747,11 +1824,11 @@
     <x v="0"/>
     <n v="20000"/>
     <x v="0"/>
-    <s v="1952-W"/>
+    <x v="18"/>
     <s v="766BC-B"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -1765,11 +1842,11 @@
     <x v="0"/>
     <n v="30000"/>
     <x v="0"/>
-    <s v="1928-W"/>
+    <x v="19"/>
     <s v="766BC-B"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -1783,11 +1860,11 @@
     <x v="0"/>
     <n v="40000"/>
     <x v="0"/>
-    <s v="1976-W"/>
+    <x v="20"/>
     <s v="766BC-B"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -1801,11 +1878,11 @@
     <x v="0"/>
     <n v="50000"/>
     <x v="0"/>
-    <s v="1964-W"/>
+    <x v="21"/>
     <s v="766BC-B"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -1819,11 +1896,11 @@
     <x v="0"/>
     <n v="60000"/>
     <x v="0"/>
-    <s v="70060"/>
+    <x v="22"/>
     <s v="766BC-B"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -1837,11 +1914,11 @@
     <x v="0"/>
     <n v="70000"/>
     <x v="0"/>
-    <s v="1896-S"/>
+    <x v="23"/>
     <s v="766BC-B"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -1855,11 +1932,11 @@
     <x v="0"/>
     <n v="80000"/>
     <x v="0"/>
-    <s v="1908-S"/>
+    <x v="24"/>
     <s v="766BC-B"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -1873,11 +1950,11 @@
     <x v="0"/>
     <n v="90000"/>
     <x v="0"/>
-    <s v="1928-S"/>
+    <x v="25"/>
     <s v="766BC-B"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -1891,11 +1968,11 @@
     <x v="0"/>
     <n v="100000"/>
     <x v="0"/>
-    <s v="70102"/>
+    <x v="13"/>
     <s v="766BC-B"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -1909,11 +1986,11 @@
     <x v="0"/>
     <n v="10000"/>
     <x v="0"/>
-    <s v="1952-W"/>
+    <x v="18"/>
     <s v="766BC-C"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -1927,11 +2004,11 @@
     <x v="0"/>
     <n v="20000"/>
     <x v="0"/>
-    <s v="1928-W"/>
+    <x v="19"/>
     <s v="766BC-C"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -1945,11 +2022,11 @@
     <x v="0"/>
     <n v="30000"/>
     <x v="0"/>
-    <s v="1976-W"/>
+    <x v="20"/>
     <s v="766BC-C"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -1963,11 +2040,11 @@
     <x v="0"/>
     <n v="40000"/>
     <x v="0"/>
-    <s v="1964-W"/>
+    <x v="21"/>
     <s v="766BC-C"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -1981,11 +2058,11 @@
     <x v="0"/>
     <n v="50000"/>
     <x v="0"/>
-    <s v="70060"/>
+    <x v="22"/>
     <s v="766BC-C"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -1999,11 +2076,11 @@
     <x v="0"/>
     <n v="10000"/>
     <x v="0"/>
-    <s v="80001"/>
+    <x v="26"/>
     <s v="8904-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -2017,11 +2094,11 @@
     <x v="0"/>
     <n v="20000"/>
     <x v="0"/>
-    <s v="80010"/>
+    <x v="27"/>
     <s v="8904-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -2035,11 +2112,11 @@
     <x v="0"/>
     <n v="30000"/>
     <x v="0"/>
-    <s v="80201"/>
+    <x v="28"/>
     <s v="8904-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -2053,11 +2130,11 @@
     <x v="0"/>
     <n v="40000"/>
     <x v="0"/>
-    <s v="80021"/>
+    <x v="29"/>
     <s v="8904-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -2071,11 +2148,11 @@
     <x v="0"/>
     <n v="50000"/>
     <x v="0"/>
-    <s v="80101"/>
+    <x v="30"/>
     <s v="8904-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -2089,11 +2166,11 @@
     <x v="0"/>
     <n v="60000"/>
     <x v="0"/>
-    <s v="80206"/>
+    <x v="31"/>
     <s v="8904-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -2107,11 +2184,11 @@
     <x v="0"/>
     <n v="70000"/>
     <x v="0"/>
-    <s v="80211"/>
+    <x v="32"/>
     <s v="8904-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -2125,11 +2202,11 @@
     <x v="0"/>
     <n v="10000"/>
     <x v="0"/>
-    <s v="80002"/>
+    <x v="33"/>
     <s v="8908-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -2143,11 +2220,11 @@
     <x v="0"/>
     <n v="20000"/>
     <x v="0"/>
-    <s v="80011"/>
+    <x v="34"/>
     <s v="8908-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -2161,11 +2238,11 @@
     <x v="0"/>
     <n v="30000"/>
     <x v="0"/>
-    <s v="80202"/>
+    <x v="35"/>
     <s v="8908-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -2179,11 +2256,11 @@
     <x v="0"/>
     <n v="40000"/>
     <x v="0"/>
-    <s v="80023"/>
+    <x v="36"/>
     <s v="8908-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -2197,11 +2274,11 @@
     <x v="0"/>
     <n v="50000"/>
     <x v="0"/>
-    <s v="80102"/>
+    <x v="37"/>
     <s v="8908-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -2215,11 +2292,11 @@
     <x v="0"/>
     <n v="60000"/>
     <x v="0"/>
-    <s v="80208"/>
+    <x v="38"/>
     <s v="8908-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -2233,11 +2310,11 @@
     <x v="0"/>
     <n v="70000"/>
     <x v="0"/>
-    <s v="80209"/>
+    <x v="39"/>
     <s v="8908-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -2251,11 +2328,11 @@
     <x v="0"/>
     <n v="80000"/>
     <x v="0"/>
-    <s v="80211"/>
+    <x v="32"/>
     <s v="8908-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -2269,11 +2346,11 @@
     <x v="0"/>
     <n v="10000"/>
     <x v="0"/>
-    <s v="80003"/>
+    <x v="40"/>
     <s v="8912-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -2287,11 +2364,11 @@
     <x v="0"/>
     <n v="20000"/>
     <x v="0"/>
-    <s v="80013"/>
+    <x v="41"/>
     <s v="8912-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -2305,11 +2382,11 @@
     <x v="0"/>
     <n v="30000"/>
     <x v="0"/>
-    <s v="80202"/>
+    <x v="35"/>
     <s v="8912-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -2323,11 +2400,11 @@
     <x v="0"/>
     <n v="40000"/>
     <x v="0"/>
-    <s v="80024"/>
+    <x v="42"/>
     <s v="8912-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -2341,11 +2418,11 @@
     <x v="0"/>
     <n v="50000"/>
     <x v="0"/>
-    <s v="80103"/>
+    <x v="43"/>
     <s v="8912-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -2359,11 +2436,11 @@
     <x v="0"/>
     <n v="60000"/>
     <x v="0"/>
-    <s v="80208"/>
+    <x v="38"/>
     <s v="8912-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -2377,11 +2454,11 @@
     <x v="0"/>
     <n v="70000"/>
     <x v="0"/>
-    <s v="80209"/>
+    <x v="39"/>
     <s v="8912-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -2395,11 +2472,11 @@
     <x v="0"/>
     <n v="80000"/>
     <x v="0"/>
-    <s v="80212"/>
+    <x v="44"/>
     <s v="8912-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -2413,11 +2490,11 @@
     <x v="0"/>
     <n v="10000"/>
     <x v="0"/>
-    <s v="80004"/>
+    <x v="45"/>
     <s v="8916-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -2431,11 +2508,11 @@
     <x v="0"/>
     <n v="20000"/>
     <x v="0"/>
-    <s v="80014"/>
+    <x v="46"/>
     <s v="8916-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -2449,11 +2526,11 @@
     <x v="0"/>
     <n v="30000"/>
     <x v="0"/>
-    <s v="80203"/>
+    <x v="47"/>
     <s v="8916-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -2467,11 +2544,11 @@
     <x v="0"/>
     <n v="40000"/>
     <x v="0"/>
-    <s v="80026"/>
+    <x v="48"/>
     <s v="8916-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -2485,11 +2562,11 @@
     <x v="0"/>
     <n v="50000"/>
     <x v="0"/>
-    <s v="80204"/>
+    <x v="49"/>
     <s v="8916-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -2503,11 +2580,11 @@
     <x v="0"/>
     <n v="60000"/>
     <x v="0"/>
-    <s v="80105"/>
+    <x v="50"/>
     <s v="8916-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -2521,11 +2598,11 @@
     <x v="0"/>
     <n v="70000"/>
     <x v="0"/>
-    <s v="80207"/>
+    <x v="51"/>
     <s v="8916-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -2539,11 +2616,11 @@
     <x v="0"/>
     <n v="80000"/>
     <x v="0"/>
-    <s v="80210"/>
+    <x v="52"/>
     <s v="8916-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -2557,11 +2634,11 @@
     <x v="0"/>
     <n v="90000"/>
     <x v="0"/>
-    <s v="80212"/>
+    <x v="44"/>
     <s v="8916-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -2575,11 +2652,11 @@
     <x v="0"/>
     <n v="100000"/>
     <x v="0"/>
-    <s v="80213"/>
+    <x v="53"/>
     <s v="8916-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -2593,11 +2670,11 @@
     <x v="0"/>
     <n v="110000"/>
     <x v="0"/>
-    <s v="80214"/>
+    <x v="54"/>
     <s v="8916-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -2611,11 +2688,11 @@
     <x v="0"/>
     <n v="10000"/>
     <x v="0"/>
-    <s v="80202"/>
+    <x v="35"/>
     <s v="8920-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -2629,11 +2706,11 @@
     <x v="0"/>
     <n v="20000"/>
     <x v="0"/>
-    <s v="80027"/>
+    <x v="55"/>
     <s v="8920-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -2647,11 +2724,11 @@
     <x v="0"/>
     <n v="30000"/>
     <x v="0"/>
-    <s v="80204"/>
+    <x v="49"/>
     <s v="8920-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -2665,11 +2742,11 @@
     <x v="0"/>
     <n v="40000"/>
     <x v="0"/>
-    <s v="80205"/>
+    <x v="56"/>
     <s v="8920-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -2683,11 +2760,11 @@
     <x v="0"/>
     <n v="50000"/>
     <x v="0"/>
-    <s v="80208"/>
+    <x v="38"/>
     <s v="8920-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -2701,11 +2778,11 @@
     <x v="0"/>
     <n v="60000"/>
     <x v="0"/>
-    <s v="80209"/>
+    <x v="39"/>
     <s v="8920-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -2719,11 +2796,11 @@
     <x v="0"/>
     <n v="70000"/>
     <x v="0"/>
-    <s v="80211"/>
+    <x v="32"/>
     <s v="8920-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -2737,11 +2814,11 @@
     <x v="0"/>
     <n v="80000"/>
     <x v="0"/>
-    <s v="80006"/>
+    <x v="57"/>
     <s v="8920-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -2755,11 +2832,11 @@
     <x v="0"/>
     <n v="10000"/>
     <x v="0"/>
-    <s v="80202"/>
+    <x v="35"/>
     <s v="8924-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -2773,11 +2850,11 @@
     <x v="0"/>
     <n v="20000"/>
     <x v="0"/>
-    <s v="80027"/>
+    <x v="55"/>
     <s v="8924-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -2791,11 +2868,11 @@
     <x v="0"/>
     <n v="30000"/>
     <x v="0"/>
-    <s v="80204"/>
+    <x v="49"/>
     <s v="8924-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -2809,11 +2886,11 @@
     <x v="0"/>
     <n v="40000"/>
     <x v="0"/>
-    <s v="80103"/>
+    <x v="43"/>
     <s v="8924-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -2827,11 +2904,11 @@
     <x v="0"/>
     <n v="50000"/>
     <x v="0"/>
-    <s v="80205"/>
+    <x v="56"/>
     <s v="8924-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -2845,11 +2922,11 @@
     <x v="0"/>
     <n v="60000"/>
     <x v="0"/>
-    <s v="80208"/>
+    <x v="38"/>
     <s v="8924-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -2863,11 +2940,11 @@
     <x v="0"/>
     <n v="70000"/>
     <x v="0"/>
-    <s v="80210"/>
+    <x v="52"/>
     <s v="8924-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -2881,11 +2958,11 @@
     <x v="0"/>
     <n v="80000"/>
     <x v="0"/>
-    <s v="80212"/>
+    <x v="44"/>
     <s v="8924-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -2899,11 +2976,11 @@
     <x v="0"/>
     <n v="90000"/>
     <x v="0"/>
-    <s v="80007"/>
+    <x v="58"/>
     <s v="8924-W"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -2917,11 +2994,11 @@
     <x v="0"/>
     <n v="10000"/>
     <x v="0"/>
-    <s v="LSU-15"/>
+    <x v="59"/>
     <s v="LS-100"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -2935,11 +3012,11 @@
     <x v="0"/>
     <n v="20000"/>
     <x v="0"/>
-    <s v="LSU-8"/>
+    <x v="60"/>
     <s v="LS-100"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -2953,11 +3030,11 @@
     <x v="0"/>
     <n v="30000"/>
     <x v="0"/>
-    <s v="LSU-4"/>
+    <x v="61"/>
     <s v="LS-100"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -2971,11 +3048,11 @@
     <x v="0"/>
     <n v="40000"/>
     <x v="0"/>
-    <s v="FF-100"/>
+    <x v="62"/>
     <s v="LS-100"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -2989,11 +3066,11 @@
     <x v="0"/>
     <n v="50000"/>
     <x v="0"/>
-    <s v="C-100"/>
+    <x v="63"/>
     <s v="LS-100"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -3007,11 +3084,11 @@
     <x v="0"/>
     <n v="60000"/>
     <x v="0"/>
-    <s v="HS-100"/>
+    <x v="64"/>
     <s v="LS-100"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="1"/>
     <x v="0"/>
     <x v="0"/>
@@ -3025,11 +3102,11 @@
     <x v="0"/>
     <n v="70000"/>
     <x v="0"/>
-    <s v="SPK-100"/>
+    <x v="65"/>
     <s v="LS-100"/>
     <x v="0"/>
-    <s v=""/>
-    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
     <n v="4"/>
     <x v="0"/>
     <x v="0"/>
@@ -3040,7 +3117,799 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="126" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="C20:C219" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="16">
+    <pivotField axis="axisRow" showAll="0">
+      <items count="67">
+        <item x="29"/>
+        <item x="34"/>
+        <item x="30"/>
+        <item x="37"/>
+        <item x="48"/>
+        <item x="43"/>
+        <item x="39"/>
+        <item x="50"/>
+        <item x="36"/>
+        <item x="55"/>
+        <item x="41"/>
+        <item x="56"/>
+        <item x="42"/>
+        <item x="46"/>
+        <item x="27"/>
+        <item x="52"/>
+        <item x="25"/>
+        <item x="16"/>
+        <item x="23"/>
+        <item x="9"/>
+        <item x="1"/>
+        <item x="59"/>
+        <item x="63"/>
+        <item x="35"/>
+        <item x="8"/>
+        <item x="4"/>
+        <item x="28"/>
+        <item x="58"/>
+        <item x="62"/>
+        <item x="6"/>
+        <item x="7"/>
+        <item x="64"/>
+        <item x="21"/>
+        <item x="20"/>
+        <item x="53"/>
+        <item x="54"/>
+        <item x="31"/>
+        <item x="51"/>
+        <item x="24"/>
+        <item x="47"/>
+        <item x="38"/>
+        <item x="60"/>
+        <item x="22"/>
+        <item x="18"/>
+        <item x="11"/>
+        <item x="13"/>
+        <item x="15"/>
+        <item x="10"/>
+        <item x="14"/>
+        <item x="17"/>
+        <item x="26"/>
+        <item x="33"/>
+        <item x="40"/>
+        <item x="45"/>
+        <item x="44"/>
+        <item x="32"/>
+        <item x="3"/>
+        <item x="5"/>
+        <item x="0"/>
+        <item x="65"/>
+        <item x="19"/>
+        <item x="57"/>
+        <item x="2"/>
+        <item x="61"/>
+        <item x="49"/>
+        <item x="12"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="67">
+        <item x="23"/>
+        <item x="17"/>
+        <item x="24"/>
+        <item x="16"/>
+        <item x="25"/>
+        <item x="19"/>
+        <item x="18"/>
+        <item x="21"/>
+        <item x="20"/>
+        <item x="9"/>
+        <item x="0"/>
+        <item x="1"/>
+        <item x="2"/>
+        <item x="3"/>
+        <item x="12"/>
+        <item x="6"/>
+        <item x="4"/>
+        <item x="5"/>
+        <item x="22"/>
+        <item x="11"/>
+        <item x="14"/>
+        <item x="13"/>
+        <item x="10"/>
+        <item x="15"/>
+        <item x="7"/>
+        <item x="8"/>
+        <item x="26"/>
+        <item x="33"/>
+        <item x="40"/>
+        <item x="45"/>
+        <item x="57"/>
+        <item x="58"/>
+        <item x="27"/>
+        <item x="34"/>
+        <item x="41"/>
+        <item x="46"/>
+        <item x="29"/>
+        <item x="36"/>
+        <item x="42"/>
+        <item x="48"/>
+        <item x="55"/>
+        <item x="30"/>
+        <item x="37"/>
+        <item x="43"/>
+        <item x="50"/>
+        <item x="28"/>
+        <item x="35"/>
+        <item x="47"/>
+        <item x="49"/>
+        <item x="56"/>
+        <item x="31"/>
+        <item x="51"/>
+        <item x="38"/>
+        <item x="39"/>
+        <item x="52"/>
+        <item x="32"/>
+        <item x="44"/>
+        <item x="53"/>
+        <item x="54"/>
+        <item x="63"/>
+        <item x="62"/>
+        <item x="64"/>
+        <item x="59"/>
+        <item x="61"/>
+        <item x="60"/>
+        <item x="65"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0">
+      <items count="2">
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0">
+      <items count="2">
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="2">
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+  </pivotFields>
+  <rowFields count="3">
+    <field x="6"/>
+    <field x="13"/>
+    <field x="0"/>
+  </rowFields>
+  <rowItems count="199">
+    <i>
+      <x/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="18"/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="49"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="38"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="17"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="16"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="60"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="43"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="32"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="33"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="19"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="58"/>
+    </i>
+    <i>
+      <x v="11"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="20"/>
+    </i>
+    <i>
+      <x v="12"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="62"/>
+    </i>
+    <i>
+      <x v="13"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="56"/>
+    </i>
+    <i>
+      <x v="14"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="65"/>
+    </i>
+    <i>
+      <x v="15"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="29"/>
+    </i>
+    <i>
+      <x v="16"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="25"/>
+    </i>
+    <i>
+      <x v="17"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="57"/>
+    </i>
+    <i>
+      <x v="18"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="42"/>
+    </i>
+    <i>
+      <x v="19"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="44"/>
+    </i>
+    <i>
+      <x v="20"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="48"/>
+    </i>
+    <i>
+      <x v="21"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="45"/>
+    </i>
+    <i>
+      <x v="22"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="47"/>
+    </i>
+    <i>
+      <x v="23"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="46"/>
+    </i>
+    <i>
+      <x v="24"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="30"/>
+    </i>
+    <i>
+      <x v="25"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="24"/>
+    </i>
+    <i>
+      <x v="26"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="50"/>
+    </i>
+    <i>
+      <x v="27"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="51"/>
+    </i>
+    <i>
+      <x v="28"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="52"/>
+    </i>
+    <i>
+      <x v="29"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="53"/>
+    </i>
+    <i>
+      <x v="30"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="61"/>
+    </i>
+    <i>
+      <x v="31"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="27"/>
+    </i>
+    <i>
+      <x v="32"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="14"/>
+    </i>
+    <i>
+      <x v="33"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="34"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="10"/>
+    </i>
+    <i>
+      <x v="35"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="13"/>
+    </i>
+    <i>
+      <x v="36"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x/>
+    </i>
+    <i>
+      <x v="37"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="38"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="12"/>
+    </i>
+    <i>
+      <x v="39"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="40"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="41"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="42"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="43"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="44"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="45"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="26"/>
+    </i>
+    <i>
+      <x v="46"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="23"/>
+    </i>
+    <i>
+      <x v="47"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="39"/>
+    </i>
+    <i>
+      <x v="48"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="64"/>
+    </i>
+    <i>
+      <x v="49"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="11"/>
+    </i>
+    <i>
+      <x v="50"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="36"/>
+    </i>
+    <i>
+      <x v="51"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="37"/>
+    </i>
+    <i>
+      <x v="52"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="40"/>
+    </i>
+    <i>
+      <x v="53"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="54"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="15"/>
+    </i>
+    <i>
+      <x v="55"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="55"/>
+    </i>
+    <i>
+      <x v="56"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="54"/>
+    </i>
+    <i>
+      <x v="57"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="34"/>
+    </i>
+    <i>
+      <x v="58"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="35"/>
+    </i>
+    <i>
+      <x v="59"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="22"/>
+    </i>
+    <i>
+      <x v="60"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="28"/>
+    </i>
+    <i>
+      <x v="61"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="31"/>
+    </i>
+    <i>
+      <x v="62"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="21"/>
+    </i>
+    <i>
+      <x v="63"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="63"/>
+    </i>
+    <i>
+      <x v="64"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="41"/>
+    </i>
+    <i>
+      <x v="65"/>
+    </i>
+    <i r="1">
+      <x/>
+    </i>
+    <i r="2">
+      <x v="59"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="126" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="C3:E8" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
   <pivotFields count="16">
     <pivotField showAll="0">
@@ -3211,6 +4080,7 @@
 <slicerCacheDefinition xmlns="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main" mc:Ignorable="x" name="Slicer_Description" sourceName="Description">
   <pivotTables>
     <pivotTable tabId="4" name="PivotTable1"/>
+    <pivotTable tabId="4" name="PivotTable2"/>
   </pivotTables>
   <data>
     <tabular pivotCacheId="1">
@@ -3583,25 +4453,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH122"/>
   <sheetViews>
-    <sheetView topLeftCell="N104" workbookViewId="0"/>
+    <sheetView topLeftCell="N2" workbookViewId="0">
+      <selection activeCell="N5" sqref="N5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="26.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.75" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.75" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.25" bestFit="1" customWidth="1"/>
-    <col min="11" max="13" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.375" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="12.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="13" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="12.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:34" hidden="1" x14ac:dyDescent="0.25">
@@ -10031,18 +10903,80 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E219"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="0" hidden="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5" customWidth="1"/>
-    <col min="4" max="4" width="14.125" customWidth="1"/>
-    <col min="5" max="5" width="9.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" customWidth="1"/>
+    <col min="6" max="6" width="20.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="16" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="27.140625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="26" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="5.140625" customWidth="1"/>
+    <col min="25" max="25" width="26" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="7.42578125" customWidth="1"/>
+    <col min="30" max="30" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="26.5703125" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="6.140625" customWidth="1"/>
+    <col min="35" max="35" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="30.7109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="31.28515625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="31.140625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="23" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="10.5703125" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="53" max="53" width="22.85546875" bestFit="1" customWidth="1"/>
+    <col min="54" max="57" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="59" max="59" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="10.42578125" bestFit="1" customWidth="1"/>
+    <col min="61" max="61" width="5.5703125" customWidth="1"/>
+    <col min="62" max="62" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="15" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="30.85546875" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="70" max="71" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" hidden="1" x14ac:dyDescent="0.25">
@@ -10117,13 +11051,1013 @@
         <v>51</v>
       </c>
     </row>
+    <row r="20" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C20" s="6" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="21" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C21" s="7" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C22" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C23" s="9" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="24" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C24" s="7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C25" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="26" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C26" s="9" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="27" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C27" s="7" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="28" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C28" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="29" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C29" s="9" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="30" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C30" s="7" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="31" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C31" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C32" s="9" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C33" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C34" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C35" s="9" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="36" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C36" s="7" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C37" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C38" s="9" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="39" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C39" s="7" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="40" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C40" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="41" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C41" s="9" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="42" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C42" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="43" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C43" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="44" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C44" s="9" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="45" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C45" s="7" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="46" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C46" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="47" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C47" s="9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="48" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C48" s="7" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="49" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C49" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="50" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C50" s="9" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="51" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C51" s="7" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="52" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C52" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="53" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C53" s="9" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="54" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C54" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="55" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C55" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="56" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C56" s="9" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="57" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C57" s="7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="58" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C58" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="59" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C59" s="9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="60" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C60" s="7" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="61" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C61" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="62" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C62" s="9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="63" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C63" s="7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C64" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="65" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C65" s="9" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="66" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C66" s="7" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="67" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C67" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="68" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C68" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="69" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C69" s="7" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="70" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C70" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="71" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C71" s="9" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="72" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C72" s="7" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="73" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C73" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="74" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C74" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="75" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C75" s="7" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="76" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C76" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="77" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C77" s="9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="78" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C78" s="7" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="79" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C79" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="80" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C80" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="81" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C81" s="7" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="82" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C82" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="83" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C83" s="9" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="84" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C84" s="7" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="85" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C85" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="86" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C86" s="9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="87" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C87" s="7" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="88" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C88" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="89" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C89" s="9" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="90" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C90" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="91" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C91" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="92" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C92" s="9" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="93" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C93" s="7" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="94" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C94" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="95" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C95" s="9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="96" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C96" s="7" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="97" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C97" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="98" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C98" s="9" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="99" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C99" s="7" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="100" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C100" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="101" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C101" s="9" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="102" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C102" s="7" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="103" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C103" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="104" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C104" s="9" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="105" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C105" s="7" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="106" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C106" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="107" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C107" s="9" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="108" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C108" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="109" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C109" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="110" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C110" s="9" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="111" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C111" s="7" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="112" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C112" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="113" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C113" s="9" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="114" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C114" s="7" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="115" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C115" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="116" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C116" s="9" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="117" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C117" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="118" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C118" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="119" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C119" s="9" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="120" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C120" s="7" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="121" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C121" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="122" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C122" s="9" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="123" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C123" s="7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="124" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C124" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="125" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C125" s="9" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="126" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C126" s="7" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="127" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C127" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="128" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C128" s="9" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="129" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C129" s="7" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="130" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C130" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="131" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C131" s="9" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="132" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C132" s="7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="133" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C133" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="134" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C134" s="9" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="135" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C135" s="7" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="136" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C136" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="137" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C137" s="9" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="138" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C138" s="7" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="139" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C139" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="140" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C140" s="9" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="141" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C141" s="7" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="142" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C142" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="143" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C143" s="9" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="144" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C144" s="7" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="145" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C145" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="146" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C146" s="9" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="147" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C147" s="7" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="148" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C148" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="149" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C149" s="9" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="150" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C150" s="7" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="151" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C151" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="152" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C152" s="9" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="153" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C153" s="7" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="154" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C154" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="155" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C155" s="9" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="156" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C156" s="7" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="157" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C157" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="158" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C158" s="9" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="159" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C159" s="7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="160" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C160" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="161" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C161" s="9" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="162" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C162" s="7" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="163" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C163" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="164" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C164" s="9" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="165" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C165" s="7" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="166" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C166" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="167" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C167" s="9" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="168" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C168" s="7" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="169" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C169" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="170" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C170" s="9" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="171" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C171" s="7" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="172" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C172" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="173" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C173" s="9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="174" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C174" s="7" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="175" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C175" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="176" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C176" s="9" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="177" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C177" s="7" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="178" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C178" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="179" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C179" s="9" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="180" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C180" s="7" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="181" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C181" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="182" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C182" s="9" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="183" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C183" s="7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="184" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C184" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="185" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C185" s="9" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="186" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C186" s="7" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="187" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C187" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="188" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C188" s="9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="189" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C189" s="7" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="190" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C190" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="191" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C191" s="9" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="192" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C192" s="7" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="193" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C193" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="194" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C194" s="9" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="195" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C195" s="7" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="196" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C196" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="197" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C197" s="9" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="198" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C198" s="7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="199" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C199" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="200" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C200" s="9" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="201" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C201" s="7" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="202" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C202" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="203" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C203" s="9" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="204" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C204" s="7" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="205" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C205" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="206" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C206" s="9" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="207" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C207" s="7" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="208" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C208" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="209" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C209" s="9" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="210" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C210" s="7" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="211" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C211" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="212" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C212" s="9" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="213" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C213" s="7" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="214" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C214" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="215" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C215" s="9" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="216" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C216" s="7" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="217" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C217" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="218" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C218" s="9" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="219" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C219" s="7" t="s">
+        <v>182</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId3"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{A8765BA9-456A-4dab-B4F3-ACF838C121DE}">
       <x14:slicerList>
-        <x14:slicer r:id="rId3"/>
+        <x14:slicer r:id="rId4"/>
       </x14:slicerList>
     </ext>
   </extLst>

</xml_diff>